<commit_message>
Made it so it would include the website name in the stats so that we can classify the data to a specific site.
</commit_message>
<xml_diff>
--- a/Data/pcap_analysis.xlsx
+++ b/Data/pcap_analysis.xlsx
@@ -11262,7 +11262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11273,94 +11273,109 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Mean Packet Size</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Median Packet Size</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Std Packet Size</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Mean Time Interval</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Median Time Interval</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Std deviation Time Interval</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Total Packets</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Total Bytes</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>blindonion</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>263.9342465753425</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>95</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>369.9997268409958</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.1043897303906116</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.01384198665618896</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.2377662349585084</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>365</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>96336</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>poop</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>141.52</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>77</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>142.1001716237887</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.2111595698765346</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.05345702171325684</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.2488049136961206</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>50</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>7076</v>
       </c>
     </row>

</xml_diff>